<commit_message>
[individual calc] update fixtures
</commit_message>
<xml_diff>
--- a/public/local/fixtures/calculator/Техническая экспертиза калькуляторы.xlsx
+++ b/public/local/fixtures/calculator/Техническая экспертиза калькуляторы.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="37580" windowHeight="21140" activeTab="1"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="37580" windowHeight="21140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Экспертиза одного здания" sheetId="4" r:id="rId1"/>
@@ -2544,7 +2544,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2716,6 +2716,7 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -18195,8 +18196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AG209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18682,6 +18683,7 @@
       <c r="B28" s="6" t="s">
         <v>456</v>
       </c>
+      <c r="C28" s="83"/>
       <c r="D28" s="68">
         <v>25000</v>
       </c>
@@ -18694,6 +18696,7 @@
       <c r="B29" s="6" t="s">
         <v>457</v>
       </c>
+      <c r="C29" s="83"/>
       <c r="D29" s="68">
         <v>25000</v>
       </c>
@@ -18706,6 +18709,7 @@
       <c r="B30" s="6" t="s">
         <v>458</v>
       </c>
+      <c r="C30" s="83"/>
       <c r="D30" s="68">
         <v>25000</v>
       </c>

</xml_diff>